<commit_message>
Team attendance [B8-G1] 04-08
Team attendance [B8-G1] 04-08
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF8F48F-CAFF-4475-8718-0BC3991D6DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A7BE62-EAA0-4077-A3C8-6BA134C46AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
   <sheets>
     <sheet name="ANG B8-G1" sheetId="1" r:id="rId1"/>
@@ -104,6 +104,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{B4E4EA40-C2E2-422C-B225-246E0B9DE3B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{7C97B06B-2C0D-4693-955C-E798301B5CE4}">
       <text>
         <r>
@@ -204,6 +228,103 @@
       </text>
     </comment>
     <comment ref="H3" authorId="0" shapeId="0" xr:uid="{BC845946-6FD6-4679-AEA5-DC38C84B37D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{CC0CD36B-31AD-4969-8150-913DFFB24473}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{0563924C-7949-47A4-BE3E-72882AE8188B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{817A552D-7701-41A3-BB40-635E530B3AAD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{8614BC10-F125-4EA1-9D91-28CBCED7A6F3}">
       <text>
         <r>
           <rPr>
@@ -232,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +383,9 @@
   </si>
   <si>
     <t>Ashwini</t>
+  </si>
+  <si>
+    <t>Priya Gawhane</t>
   </si>
 </sst>
 </file>
@@ -657,9 +781,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -698,6 +822,9 @@
       <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -725,6 +852,9 @@
       <c r="H2" t="s">
         <v>1</v>
       </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -751,10 +881,37 @@
       <c r="H3" t="s">
         <v>1</v>
       </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>45142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Team Everyday Attendance[B8-G1] 07-08-2023
Team Everyday Attendance[B8-G1] 07-08-2023
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A7BE62-EAA0-4077-A3C8-6BA134C46AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FB7F17-C278-4CD8-AD13-5A57CF242BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -348,12 +348,87 @@
         </r>
       </text>
     </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{94955947-D362-4A1B-AFA3-26C58C241D9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{59B8E493-D9A7-4D79-8C70-6C1AB976A9B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{0CC40DE6-3292-4B87-9EB5-D0FB7C805A3B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -779,11 +854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -914,6 +989,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>45145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance [B8-G1] 09-Aug
Team Attendance [B8-G1] 09-Aug
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E09DF4-809F-461C-AA6C-E6E5331B48D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689BA099-4AB4-4B35-9581-0A2019749C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -544,12 +544,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{80FB8002-987C-40BF-8944-1CB9069776EA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{58E8AC22-438A-4EB8-8F4B-6BD50978CBB2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{A6CAB027-D1B1-4094-A046-CD912AF139BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -975,11 +1047,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1168,6 +1240,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>45147</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance [B8-G1] 10-Aug.
Team Attendance [B8-G1] 10-Aug.
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689BA099-4AB4-4B35-9581-0A2019749C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02D5253-71C6-4399-A3C5-27990CEBAB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
   <sheets>
     <sheet name="ANG B8-G1" sheetId="1" r:id="rId1"/>
@@ -616,12 +616,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{8523635A-E0DC-4ABA-BAB1-F88F2AA8D88C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{039AEA5E-29C5-43E8-94B2-BD47599E09FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{5C6D3D58-D1CA-4CEE-AE53-CC65F9C7DF8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{B7768957-2AE2-4D07-B4F1-78A6ED2E09FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1047,11 +1143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1269,6 +1365,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>45148</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance B8-G1 16-AUG
Team Attendance B8-G1 16-AUG
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C688146C-6F5F-4D08-B7D5-71681105E039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62CE635-EDA0-4B86-A5EA-5DE7AA0A124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
   <sheets>
     <sheet name="ANG B8-G1" sheetId="1" r:id="rId1"/>
@@ -832,12 +832,132 @@
         </r>
       </text>
     </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{0AB14F20-9B20-4DF2-A816-FFB854E38786}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not well health issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{BCE6A148-E7AE-455F-A78B-0559C525E2D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{1FE0C7E9-01A1-4FD5-8469-3DA10AE5FB90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{FC460FF4-14B0-4F4C-B49D-AF22D96B5868}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{B0565657-8B0E-480A-B653-E21960C233F3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1263,11 +1383,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1543,6 +1663,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>45154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance [B8-G1] 17-Aug
Team Attendance [B8-G1] 17-Aug
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62CE635-EDA0-4B86-A5EA-5DE7AA0A124F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36FF8B2-828E-42D4-8D2E-A3FEBAE9913A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -952,12 +952,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{308E6F24-E57D-4A90-95B6-9F10066AADC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{DA813C07-1025-43F9-A1C2-89AF178B9003}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{CD3FB170-B121-4F38-9C15-F46E05942777}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{C9A5CB4E-AC2C-41CA-B467-2B0C326BF1A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1383,11 +1479,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1692,6 +1788,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>45155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance [B8-G1] 22-Aug
Team Attendance [B8-G1] 22-Aug
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A6B410-BAE5-4068-A474-D8912AC1E97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEAB06E-5A02-44AC-8ED3-1A15F18BA998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7270" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
   <sheets>
     <sheet name="ANG B8-G1" sheetId="1" r:id="rId1"/>
@@ -1144,12 +1144,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{EAC6B3CB-3216-405B-A8B7-1DB16B3B8BF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{A3680050-2840-4621-80EA-05215278785B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{389BF5BC-8B89-4A8A-B04A-6DB2A796EA6D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{397CD959-C7A2-4175-B820-B1D6ED9A85E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1575,11 +1671,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1942,6 +2038,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>45160</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance [B8-G1] 23-Aug
Team Attendance [B8-G1] 23-Aug
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEAB06E-5A02-44AC-8ED3-1A15F18BA998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46DA4CC-FE48-44AD-A8A6-1259539158E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1240,12 +1240,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{C133BA56-945E-4FFC-B292-3835473F5D4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{F1D30467-0466-41E8-A66C-242F26C9AD96}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{3097027D-5D41-48C2-84C7-F92807E385D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{E8596D90-00E6-4CA7-9A0E-03F42B4826CA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1671,11 +1767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2067,6 +2163,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>45161</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
TeamAttendance B8-G1 26 -AUG
TeamAttendance B8-G1 26 -AUG
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46DA4CC-FE48-44AD-A8A6-1259539158E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA55D907-A05E-4713-87F5-41862DCBC980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1336,12 +1336,133 @@
         </r>
       </text>
     </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{DD217D58-ACE3-4613-9893-2F4F069D2A4E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+college exam
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{EF48D2D1-EB42-49E8-98B7-A470F5CC9BA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{8C2AF6D5-09EE-41B4-A462-0D8C68796264}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{2CF1F923-0A0F-4F9B-9CE4-17E0AB50DD20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{AF23ECAF-8D21-4930-B349-80B16A217880}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1468,6 +1589,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1767,11 +1892,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2192,6 +2317,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>45164</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance 5-sept B8-G1
Team Attendance 5-sept B8-G1
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA55D907-A05E-4713-87F5-41862DCBC980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6FDC6-FAEB-449E-8CA4-59144DCF67E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1457,12 +1457,180 @@
         </r>
       </text>
     </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{74911A9F-D3AD-4160-B22A-D9F8194D019C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{A024AFEC-3CAC-49F4-875E-85F21CC5DD72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{0E840432-2408-4420-968C-E94FAFD4FA69}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{31A395B5-9A7A-4CCB-A2E8-447A2CCDFC62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{A7F35127-E53F-46B2-989A-13294E28453D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{4F29B785-F50B-4FB2-B9C7-C6F2F65B15AC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{DF1BF161-0CBC-4B55-87F5-ED996E94D05B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -1589,10 +1757,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1892,11 +2056,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2346,6 +2510,64 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>45173</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>45174</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance G1-B8 06-Sept
Team Attendance G1-B8 06-Sept
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\React\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B6FDC6-FAEB-449E-8CA4-59144DCF67E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC26223-BD94-4BE4-AE46-ACE6961B6E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1625,12 +1625,132 @@
         </r>
       </text>
     </comment>
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{035A1F02-9886-43A5-A2F2-94A99E92EB1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{4DB4DCAD-FADB-4413-8E39-0B5F569E17DF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{0811B579-2DB4-4932-BD8D-6E5E8A629ACA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{5CA6D11A-9AF3-43DF-B17E-0F27F48869ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{DD0B4049-ABB7-4E56-B2FA-A726EF0865A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>RENUKA:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -2056,11 +2176,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2568,6 +2688,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="7">
+        <v>45175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>